<commit_message>
fixed subheading function and updated affected datasets
</commit_message>
<xml_diff>
--- a/data/APR_dictionary.xlsx
+++ b/data/APR_dictionary.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="APR_dictionary" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">APR_dictionary!$A$1:$G$70</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -1386,8 +1389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2911,6 +2914,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G70"/>
   <sortState ref="A2:H70">
     <sortCondition ref="A2:A70"/>
   </sortState>

</xml_diff>